<commit_message>
sort of one i think
</commit_message>
<xml_diff>
--- a/cpsc416-assignment2/results.xlsx
+++ b/cpsc416-assignment2/results.xlsx
@@ -309,16 +309,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -664,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C1" sqref="B1:C11"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>